<commit_message>
changes for AC Programs
</commit_message>
<xml_diff>
--- a/★結果ビューア/計算結果Viewer_換気_v1.0.xlsx
+++ b/★結果ビューア/計算結果Viewer_換気_v1.0.xlsx
@@ -1269,6 +1269,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1280,12 +1286,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1655,62 +1655,62 @@
       <c r="F2" s="20"/>
     </row>
     <row r="4" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="26" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="27">
         <v>3.45746666666667</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="27">
         <v>5.8235921621469899E-2</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="27">
         <v>33744.874666666699</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="27">
         <v>568.38259502554604</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="27">
         <v>0.750862305555556</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="27">
         <v>1.26471670128947E-2</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="27">
         <v>7328.4161022222197</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="27">
         <v>123.436350045852</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="31">
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="27">
         <f>E5/E6</f>
         <v>4.6046613887595766</v>
       </c>
@@ -1731,7 +1731,7 @@
   <dimension ref="A1:Y499"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A6" sqref="A6:X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1757,40 +1757,40 @@
       <c r="F1" s="20"/>
     </row>
     <row r="2" spans="1:25" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="27" t="s">
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="29"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="31"/>
       <c r="U2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="V2" s="26" t="s">
+      <c r="V2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="26"/>
-      <c r="X2" s="26"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
     </row>
     <row r="3" spans="1:25" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
@@ -2334,7 +2334,7 @@
         <v>29</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C11" s="24" t="s">
         <v>44</v>
@@ -2343,7 +2343,7 @@
         <v>25</v>
       </c>
       <c r="E11" s="6">
-        <v>11.85</v>
+        <v>13</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>39</v>
@@ -2365,7 +2365,7 @@
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="7">
-        <v>4.2194000000000003</v>
+        <v>3.8462000000000001</v>
       </c>
       <c r="P11" s="7">
         <v>2.7778</v>
@@ -2389,10 +2389,10 @@
         <v>2038.5387000000001</v>
       </c>
       <c r="W11" s="15">
-        <v>1006.5285</v>
+        <v>1104.2084</v>
       </c>
       <c r="X11" s="16">
-        <v>2.0253000000000001</v>
+        <v>1.8462000000000001</v>
       </c>
       <c r="Y11" s="19"/>
     </row>
@@ -2401,7 +2401,7 @@
         <v>29</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>44</v>
@@ -2410,7 +2410,7 @@
         <v>25</v>
       </c>
       <c r="E12" s="6">
-        <v>13</v>
+        <v>11.85</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>39</v>
@@ -2432,7 +2432,7 @@
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="7">
-        <v>3.8462000000000001</v>
+        <v>4.2194000000000003</v>
       </c>
       <c r="P12" s="7">
         <v>2.7778</v>
@@ -2456,10 +2456,10 @@
         <v>2038.5387000000001</v>
       </c>
       <c r="W12" s="15">
-        <v>1104.2084</v>
+        <v>1006.5285</v>
       </c>
       <c r="X12" s="16">
-        <v>1.8462000000000001</v>
+        <v>2.0253000000000001</v>
       </c>
       <c r="Y12" s="19"/>
     </row>

</xml_diff>